<commit_message>
Rearranged headers to be similar to PrePrints
</commit_message>
<xml_diff>
--- a/data_paper_Greek.xlsx
+++ b/data_paper_Greek.xlsx
@@ -1,18 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/onat/Documents/ornament_symmgroups/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="12480" yWindow="3120" windowWidth="19500" windowHeight="19160"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>BuSel G</t>
   </si>
@@ -29,9 +44,6 @@
     <t>Selçuk</t>
   </si>
   <si>
-    <t>Ispanya</t>
-  </si>
-  <si>
     <t>Yunan?</t>
   </si>
   <si>
@@ -105,41 +117,40 @@
   </si>
   <si>
     <t>61tane</t>
+  </si>
+  <si>
+    <t>Andalousia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="0.0000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color indexed="9"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <b val="1"/>
+      <u/>
       <sz val="10"/>
-      <color indexed="8"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -181,69 +192,130 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellStyleXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ff003366"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="000000D4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -369,7 +441,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -378,7 +450,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -387,7 +459,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -461,7 +533,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -469,7 +541,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -488,7 +560,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -518,7 +590,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -544,7 +616,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -570,7 +642,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -596,7 +668,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -622,7 +694,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -648,7 +720,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -674,7 +746,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -700,7 +772,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -726,7 +798,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -739,9 +811,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -756,7 +834,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -764,7 +842,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -783,7 +861,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -809,7 +887,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -835,7 +913,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -861,7 +939,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -887,7 +965,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -913,7 +991,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -939,7 +1017,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -965,7 +1043,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -991,7 +1069,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1017,7 +1095,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1030,9 +1108,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1046,7 +1130,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1065,7 +1149,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1095,7 +1179,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1121,7 +1205,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1147,7 +1231,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1173,7 +1257,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1199,7 +1283,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1225,7 +1309,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1251,7 +1335,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1277,7 +1361,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1303,7 +1387,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1316,58 +1400,65 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="8" width="10.8516" style="1" customWidth="1"/>
-    <col min="9" max="256" width="10.8516" style="1" customWidth="1"/>
+    <col min="1" max="8" width="10.83203125" style="1" customWidth="1"/>
+    <col min="9" max="259" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s" s="3">
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s" s="3">
+      <c r="G1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s" s="3">
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="4">
-        <v>7</v>
-      </c>
       <c r="B2" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5">
         <v>0</v>
@@ -1382,15 +1473,15 @@
         <v>0.27</v>
       </c>
       <c r="G2" s="5">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H2" s="5">
-        <v>9.800000000000001</v>
-      </c>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>8</v>
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
@@ -1402,7 +1493,7 @@
         <v>9.65</v>
       </c>
       <c r="E3" s="5">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F3" s="5">
         <v>0</v>
@@ -1414,12 +1505,12 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="4">
-        <v>9</v>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B4" s="5">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C4" s="5">
         <v>0</v>
@@ -1434,15 +1525,15 @@
         <v>0</v>
       </c>
       <c r="G4" s="5">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="H4" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="4">
-        <v>10</v>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -1451,13 +1542,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="5">
-        <v>4.39</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="E5" s="5">
         <v>2.4</v>
       </c>
       <c r="F5" s="5">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
@@ -1466,12 +1557,12 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="4">
-        <v>11</v>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B6" s="5">
-        <v>2.4</v>
+        <v>1</v>
       </c>
       <c r="C6" s="5">
         <v>3.6</v>
@@ -1483,21 +1574,21 @@
         <v>0</v>
       </c>
       <c r="F6" s="5">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G6" s="5">
-        <v>1</v>
+        <v>2.4</v>
       </c>
       <c r="H6" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="4">
-        <v>12</v>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B7" s="5">
-        <v>6.4</v>
+        <v>1.9419999999999999</v>
       </c>
       <c r="C7" s="5">
         <v>5.78</v>
@@ -1509,21 +1600,21 @@
         <v>5.7</v>
       </c>
       <c r="F7" s="5">
-        <v>8.789999999999999</v>
+        <v>8.7899999999999991</v>
       </c>
       <c r="G7" s="5">
-        <v>1.942</v>
+        <v>6.4</v>
       </c>
       <c r="H7" s="5">
         <v>6.6</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="4">
-        <v>13</v>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B8" s="5">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C8" s="5">
         <v>0.44</v>
@@ -1538,18 +1629,18 @@
         <v>0.82</v>
       </c>
       <c r="G8" s="5">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="H8" s="5">
         <v>1.6</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="4">
-        <v>14</v>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B9" s="5">
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="C9" s="5">
         <v>0</v>
@@ -1561,21 +1652,21 @@
         <v>0.8</v>
       </c>
       <c r="F9" s="5">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G9" s="5">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="H9" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="4">
-        <v>15</v>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B10" s="5">
-        <v>11.2</v>
+        <v>1.9419999999999999</v>
       </c>
       <c r="C10" s="5">
         <v>12.89</v>
@@ -1590,18 +1681,18 @@
         <v>8.52</v>
       </c>
       <c r="G10" s="5">
-        <v>1.942</v>
+        <v>11.2</v>
       </c>
       <c r="H10" s="5">
         <v>6.6</v>
       </c>
     </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="4">
-        <v>16</v>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="5">
         <v>0</v>
@@ -1616,44 +1707,44 @@
         <v>0.82</v>
       </c>
       <c r="G11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="4">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="4">
-        <v>18</v>
-      </c>
       <c r="B13" s="5">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="C13" s="5">
         <v>0.44</v>
@@ -1668,21 +1759,21 @@
         <v>1.92</v>
       </c>
       <c r="G13" s="5">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="H13" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" t="s" s="4">
-        <v>19</v>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B14" s="5">
-        <v>9.6</v>
+        <v>27.184000000000001</v>
       </c>
       <c r="C14" s="5">
-        <v>4.44</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="D14" s="5">
         <v>1.75</v>
@@ -1694,24 +1785,24 @@
         <v>8.24</v>
       </c>
       <c r="G14" s="5">
-        <v>27.184</v>
+        <v>9.6</v>
       </c>
       <c r="H14" s="5">
         <v>1.6</v>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="4">
-        <v>20</v>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B15" s="5">
-        <v>25.6</v>
+        <v>51.46</v>
       </c>
       <c r="C15" s="5">
         <v>28.89</v>
       </c>
       <c r="D15" s="5">
-        <v>35.09</v>
+        <v>35.090000000000003</v>
       </c>
       <c r="E15" s="5">
         <v>54.5</v>
@@ -1720,18 +1811,18 @@
         <v>27.75</v>
       </c>
       <c r="G15" s="5">
-        <v>51.46</v>
+        <v>25.6</v>
       </c>
       <c r="H15" s="5">
         <v>62.3</v>
       </c>
     </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="4">
-        <v>21</v>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="B16" s="5">
-        <v>12.8</v>
+        <v>5.83</v>
       </c>
       <c r="C16" s="5">
         <v>5.33</v>
@@ -1740,27 +1831,27 @@
         <v>11.4</v>
       </c>
       <c r="E16" s="5">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F16" s="5">
         <v>5.22</v>
       </c>
       <c r="G16" s="5">
-        <v>5.83</v>
+        <v>12.8</v>
       </c>
       <c r="H16" s="5">
         <v>6.6</v>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1">
-      <c r="A17" t="s" s="4">
-        <v>22</v>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B17" s="5">
-        <v>8</v>
+        <v>2.9</v>
       </c>
       <c r="C17" s="5">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D17" s="5">
         <v>0.88</v>
@@ -1772,18 +1863,18 @@
         <v>7.97</v>
       </c>
       <c r="G17" s="5">
-        <v>2.9</v>
+        <v>8</v>
       </c>
       <c r="H17" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="4">
-        <v>23</v>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B18" s="5">
-        <v>16.8</v>
+        <v>5.83</v>
       </c>
       <c r="C18" s="5">
         <v>33.78</v>
@@ -1798,13 +1889,13 @@
         <v>27.47</v>
       </c>
       <c r="G18" s="5">
-        <v>5.83</v>
+        <v>16.8</v>
       </c>
       <c r="H18" s="5">
         <v>1.6</v>
       </c>
     </row>
-    <row r="19" ht="15" customHeight="1">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1814,21 +1905,21 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" ht="15" customHeight="1">
-      <c r="A20" t="s" s="4">
-        <v>24</v>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B20" s="5">
         <f>SUM(B2:B18)</f>
-        <v>100</v>
+        <v>100.08799999999999</v>
       </c>
       <c r="C20" s="5">
         <f>SUM(C2:C18)</f>
-        <v>99.99000000000001</v>
+        <v>99.990000000000009</v>
       </c>
       <c r="D20" s="5">
-        <f>SUM(D2:D18)</f>
-        <v>100.01</v>
+        <f t="shared" ref="D20" si="0">SUM(D2:D18)</f>
+        <v>100.00999999999999</v>
       </c>
       <c r="E20" s="5">
         <f>SUM(E2:E18)</f>
@@ -1836,42 +1927,42 @@
       </c>
       <c r="F20" s="5">
         <f>SUM(F2:F18)</f>
-        <v>99.99000000000001</v>
+        <v>99.990000000000009</v>
       </c>
       <c r="G20" s="5">
         <f>SUM(G2:G18)</f>
-        <v>100.088</v>
+        <v>100</v>
       </c>
       <c r="H20" s="5">
         <f>SUM(H2:H18)</f>
-        <v>99.89999999999999</v>
-      </c>
-    </row>
-    <row r="21" ht="15" customHeight="1">
+        <v>99.899999999999991</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="7"/>
-      <c r="B21" t="s" s="8">
+      <c r="B21" s="6"/>
+      <c r="C21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C21" t="s" s="9">
+      <c r="D21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D21" t="s" s="9">
+      <c r="E21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E21" t="s" s="9">
+      <c r="F21" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F21" t="s" s="9">
+      <c r="G21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="G21" s="6"/>
-      <c r="H21" t="s" s="8">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="92" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup scale="92" orientation="landscape"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Verdana,Regular"&amp;10&amp;K00336618 Ekim 2020 Yunan eklendi</oddHeader>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>

</xml_diff>